<commit_message>
Make data in Excel file more readable for future onlookers.
</commit_message>
<xml_diff>
--- a/Mathematics and Calculations/Fuel Consumption Mapping.xlsx
+++ b/Mathematics and Calculations/Fuel Consumption Mapping.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Games\GTA V\Scripting\Traction Control\Mathematics and Calculations\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Games\GTA V\Scripting\Fuel\Mathematics and Calculations\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD81453F-73B9-4297-9F9A-405F425248B2}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="9450"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="152511"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,18 +25,33 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="7">
   <si>
     <t>x</t>
   </si>
   <si>
     <t>y</t>
   </si>
+  <si>
+    <t>Desired MPG</t>
+  </si>
+  <si>
+    <t>Speed (mph)</t>
+  </si>
+  <si>
+    <t>Dataset 3</t>
+  </si>
+  <si>
+    <t>Dataset 2</t>
+  </si>
+  <si>
+    <t>Dataset 1</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -66,8 +81,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -86,7 +107,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -100,7 +121,36 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Fuel</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Economy vs. Speed</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -176,7 +226,6 @@
             <c:dispRSqr val="0"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
-              <c:layout/>
               <c:numFmt formatCode="General" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
@@ -209,7 +258,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$E$7:$E$15</c:f>
+              <c:f>Sheet1!$E$8:$E$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -245,7 +294,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$F$7:$F$15</c:f>
+              <c:f>Sheet1!$F$8:$F$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -280,6 +329,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-5E3F-4E9D-AF5D-2207FDCC2258}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -462,7 +516,7 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -476,7 +530,31 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Fuel Economy vs. Speed</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -590,7 +668,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$P$7:$P$21</c:f>
+              <c:f>Sheet1!$P$8:$P$22</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
@@ -641,7 +719,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$Q$7:$Q$21</c:f>
+              <c:f>Sheet1!$Q$8:$Q$22</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
@@ -691,6 +769,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-4BCB-44ED-A1EC-949FC8E8BFCF}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -873,7 +956,7 @@
 </file>
 
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -887,7 +970,31 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Fuel Economy vs. Speed</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1001,7 +1108,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$P$26:$P$40</c:f>
+              <c:f>Sheet1!$P$27:$P$41</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
@@ -1046,7 +1153,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$Q$26:$Q$40</c:f>
+              <c:f>Sheet1!$Q$27:$Q$41</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
@@ -1090,6 +1197,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-C9CA-4B70-A313-5FBCEEABE67A}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -2945,18 +3057,24 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>214312</xdr:colOff>
-      <xdr:row>7</xdr:row>
+      <xdr:row>8</xdr:row>
       <xdr:rowOff>161925</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
       <xdr:colOff>519112</xdr:colOff>
-      <xdr:row>22</xdr:row>
+      <xdr:row>23</xdr:row>
       <xdr:rowOff>47625</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -2975,18 +3093,24 @@
     <xdr:from>
       <xdr:col>18</xdr:col>
       <xdr:colOff>209550</xdr:colOff>
-      <xdr:row>5</xdr:row>
+      <xdr:row>6</xdr:row>
       <xdr:rowOff>142875</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>25</xdr:col>
       <xdr:colOff>514350</xdr:colOff>
-      <xdr:row>20</xdr:row>
+      <xdr:row>21</xdr:row>
       <xdr:rowOff>28575</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -3005,18 +3129,24 @@
     <xdr:from>
       <xdr:col>18</xdr:col>
       <xdr:colOff>242887</xdr:colOff>
-      <xdr:row>22</xdr:row>
+      <xdr:row>23</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>25</xdr:col>
       <xdr:colOff>547687</xdr:colOff>
-      <xdr:row>36</xdr:row>
+      <xdr:row>37</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -3296,300 +3426,347 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="E6:Q37"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="E5:Q38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I9" workbookViewId="0">
-      <selection activeCell="Q31" sqref="Q31"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="R15" sqref="R15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="6" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="12.42578125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
+    <row r="5" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F5" s="2"/>
+      <c r="P5" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q5" s="2"/>
+    </row>
     <row r="6" spans="5:17" x14ac:dyDescent="0.25">
       <c r="E6" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F6" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P6" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="Q6" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="5:17" x14ac:dyDescent="0.25">
-      <c r="E7">
-        <v>5</v>
-      </c>
-      <c r="F7">
-        <v>5</v>
-      </c>
-      <c r="P7">
-        <v>25</v>
-      </c>
-      <c r="Q7">
-        <v>25</v>
+      <c r="E7" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="P7" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q7" s="1" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="5:17" x14ac:dyDescent="0.25">
-      <c r="E8">
-        <v>30</v>
-      </c>
-      <c r="F8">
-        <v>20</v>
-      </c>
-      <c r="P8">
-        <v>0</v>
-      </c>
-      <c r="Q8">
-        <v>3</v>
+      <c r="E8" s="1">
+        <v>5</v>
+      </c>
+      <c r="F8" s="1">
+        <v>5</v>
+      </c>
+      <c r="P8" s="1">
+        <v>25</v>
+      </c>
+      <c r="Q8" s="1">
+        <v>25</v>
       </c>
     </row>
     <row r="9" spans="5:17" x14ac:dyDescent="0.25">
-      <c r="E9">
-        <v>50</v>
-      </c>
-      <c r="F9">
-        <v>15</v>
-      </c>
-      <c r="P9">
-        <v>12</v>
-      </c>
-      <c r="Q9">
-        <v>9</v>
+      <c r="E9" s="1">
+        <v>30</v>
+      </c>
+      <c r="F9" s="1">
+        <v>20</v>
+      </c>
+      <c r="P9" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q9" s="1">
+        <v>3</v>
       </c>
     </row>
     <row r="10" spans="5:17" x14ac:dyDescent="0.25">
-      <c r="E10">
-        <v>100</v>
-      </c>
-      <c r="F10">
-        <v>0</v>
-      </c>
-      <c r="P10">
-        <v>5</v>
-      </c>
-      <c r="Q10">
-        <v>5</v>
+      <c r="E10" s="1">
+        <v>50</v>
+      </c>
+      <c r="F10" s="1">
+        <v>15</v>
+      </c>
+      <c r="P10" s="1">
+        <v>12</v>
+      </c>
+      <c r="Q10" s="1">
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="5:17" x14ac:dyDescent="0.25">
-      <c r="E11">
-        <v>20</v>
-      </c>
-      <c r="F11">
-        <v>19.59</v>
-      </c>
-      <c r="P11">
-        <v>50</v>
-      </c>
-      <c r="Q11">
-        <v>15</v>
+      <c r="E11" s="1">
+        <v>100</v>
+      </c>
+      <c r="F11" s="1">
+        <v>0</v>
+      </c>
+      <c r="P11" s="1">
+        <v>5</v>
+      </c>
+      <c r="Q11" s="1">
+        <v>5</v>
       </c>
     </row>
     <row r="12" spans="5:17" x14ac:dyDescent="0.25">
-      <c r="E12">
-        <v>10</v>
-      </c>
-      <c r="F12">
-        <v>12</v>
-      </c>
-      <c r="P12">
-        <v>75</v>
-      </c>
-      <c r="Q12">
-        <v>7</v>
+      <c r="E12" s="1">
+        <v>20</v>
+      </c>
+      <c r="F12" s="1">
+        <v>19.59</v>
+      </c>
+      <c r="P12" s="1">
+        <v>50</v>
+      </c>
+      <c r="Q12" s="1">
+        <v>15</v>
       </c>
     </row>
     <row r="13" spans="5:17" x14ac:dyDescent="0.25">
-      <c r="E13">
-        <v>0</v>
-      </c>
-      <c r="F13">
-        <v>3</v>
-      </c>
-      <c r="P13">
-        <v>90</v>
-      </c>
-      <c r="Q13">
-        <v>5</v>
+      <c r="E13" s="1">
+        <v>10</v>
+      </c>
+      <c r="F13" s="1">
+        <v>12</v>
+      </c>
+      <c r="P13" s="1">
+        <v>75</v>
+      </c>
+      <c r="Q13" s="1">
+        <v>7</v>
       </c>
     </row>
     <row r="14" spans="5:17" x14ac:dyDescent="0.25">
-      <c r="E14">
-        <v>75</v>
-      </c>
-      <c r="F14">
-        <v>6</v>
-      </c>
-      <c r="P14">
-        <v>100</v>
-      </c>
-      <c r="Q14">
-        <v>4</v>
+      <c r="E14" s="1">
+        <v>0</v>
+      </c>
+      <c r="F14" s="1">
+        <v>3</v>
+      </c>
+      <c r="P14" s="1">
+        <v>90</v>
+      </c>
+      <c r="Q14" s="1">
+        <v>5</v>
       </c>
     </row>
     <row r="15" spans="5:17" x14ac:dyDescent="0.25">
-      <c r="E15">
-        <v>90</v>
-      </c>
-      <c r="F15">
-        <v>2</v>
-      </c>
-      <c r="P15">
-        <v>110</v>
-      </c>
-      <c r="Q15">
-        <v>3</v>
+      <c r="E15" s="1">
+        <v>75</v>
+      </c>
+      <c r="F15" s="1">
+        <v>6</v>
+      </c>
+      <c r="P15" s="1">
+        <v>100</v>
+      </c>
+      <c r="Q15" s="1">
+        <v>4</v>
       </c>
     </row>
     <row r="16" spans="5:17" x14ac:dyDescent="0.25">
-      <c r="P16">
-        <v>120</v>
-      </c>
-      <c r="Q16">
+      <c r="E16" s="1">
+        <v>90</v>
+      </c>
+      <c r="F16" s="1">
         <v>2</v>
+      </c>
+      <c r="P16" s="1">
+        <v>110</v>
+      </c>
+      <c r="Q16" s="1">
+        <v>3</v>
       </c>
     </row>
     <row r="17" spans="16:17" x14ac:dyDescent="0.25">
-      <c r="P17">
-        <v>130</v>
-      </c>
-      <c r="Q17">
-        <v>1.5</v>
+      <c r="P17" s="1">
+        <v>120</v>
+      </c>
+      <c r="Q17" s="1">
+        <v>2</v>
       </c>
     </row>
     <row r="18" spans="16:17" x14ac:dyDescent="0.25">
-      <c r="P18">
-        <v>20</v>
-      </c>
-      <c r="Q18">
-        <v>19</v>
+      <c r="P18" s="1">
+        <v>130</v>
+      </c>
+      <c r="Q18" s="1">
+        <v>1.5</v>
       </c>
     </row>
     <row r="19" spans="16:17" x14ac:dyDescent="0.25">
-      <c r="P19">
-        <v>140</v>
-      </c>
-      <c r="Q19">
-        <v>1.5</v>
+      <c r="P19" s="1">
+        <v>20</v>
+      </c>
+      <c r="Q19" s="1">
+        <v>19</v>
       </c>
     </row>
     <row r="20" spans="16:17" x14ac:dyDescent="0.25">
-      <c r="P20">
+      <c r="P20" s="1">
+        <v>140</v>
+      </c>
+      <c r="Q20" s="1">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="21" spans="16:17" x14ac:dyDescent="0.25">
+      <c r="P21" s="1">
         <v>150</v>
       </c>
-      <c r="Q20">
+      <c r="Q21" s="1">
         <v>1.5</v>
       </c>
+    </row>
+    <row r="24" spans="16:17" x14ac:dyDescent="0.25">
+      <c r="P24" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q24" s="2"/>
     </row>
     <row r="25" spans="16:17" x14ac:dyDescent="0.25">
       <c r="P25" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="Q25" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="26" spans="16:17" x14ac:dyDescent="0.25">
-      <c r="P26">
+      <c r="P26" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="Q26">
-        <v>3</v>
+      <c r="Q26" s="1" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="27" spans="16:17" x14ac:dyDescent="0.25">
-      <c r="P27">
-        <v>5</v>
-      </c>
-      <c r="Q27">
-        <v>8</v>
+      <c r="P27" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q27" s="1">
+        <v>3</v>
       </c>
     </row>
     <row r="28" spans="16:17" x14ac:dyDescent="0.25">
-      <c r="P28">
-        <v>28</v>
-      </c>
-      <c r="Q28">
-        <v>20</v>
+      <c r="P28" s="1">
+        <v>5</v>
+      </c>
+      <c r="Q28" s="1">
+        <v>8</v>
       </c>
     </row>
     <row r="29" spans="16:17" x14ac:dyDescent="0.25">
-      <c r="P29">
-        <v>15</v>
-      </c>
-      <c r="Q29">
-        <v>15</v>
+      <c r="P29" s="1">
+        <v>28</v>
+      </c>
+      <c r="Q29" s="1">
+        <v>20</v>
       </c>
     </row>
     <row r="30" spans="16:17" x14ac:dyDescent="0.25">
-      <c r="P30">
-        <v>40</v>
-      </c>
-      <c r="Q30">
-        <v>16</v>
+      <c r="P30" s="1">
+        <v>15</v>
+      </c>
+      <c r="Q30" s="1">
+        <v>15</v>
       </c>
     </row>
     <row r="31" spans="16:17" x14ac:dyDescent="0.25">
-      <c r="P31">
-        <v>50</v>
-      </c>
-      <c r="Q31">
-        <v>13</v>
+      <c r="P31" s="1">
+        <v>40</v>
+      </c>
+      <c r="Q31" s="1">
+        <v>16</v>
       </c>
     </row>
     <row r="32" spans="16:17" x14ac:dyDescent="0.25">
-      <c r="P32">
-        <v>60</v>
-      </c>
-      <c r="Q32">
-        <v>11</v>
+      <c r="P32" s="1">
+        <v>50</v>
+      </c>
+      <c r="Q32" s="1">
+        <v>13</v>
       </c>
     </row>
     <row r="33" spans="16:17" x14ac:dyDescent="0.25">
-      <c r="P33">
-        <v>70</v>
-      </c>
-      <c r="Q33">
-        <v>9</v>
+      <c r="P33" s="1">
+        <v>60</v>
+      </c>
+      <c r="Q33" s="1">
+        <v>11</v>
       </c>
     </row>
     <row r="34" spans="16:17" x14ac:dyDescent="0.25">
-      <c r="P34">
-        <v>80</v>
-      </c>
-      <c r="Q34">
-        <v>7</v>
+      <c r="P34" s="1">
+        <v>70</v>
+      </c>
+      <c r="Q34" s="1">
+        <v>9</v>
       </c>
     </row>
     <row r="35" spans="16:17" x14ac:dyDescent="0.25">
-      <c r="P35">
-        <v>90</v>
-      </c>
-      <c r="Q35">
-        <v>5</v>
+      <c r="P35" s="1">
+        <v>80</v>
+      </c>
+      <c r="Q35" s="1">
+        <v>7</v>
       </c>
     </row>
     <row r="36" spans="16:17" x14ac:dyDescent="0.25">
-      <c r="P36">
-        <v>100</v>
-      </c>
-      <c r="Q36">
-        <v>4</v>
+      <c r="P36" s="1">
+        <v>90</v>
+      </c>
+      <c r="Q36" s="1">
+        <v>5</v>
       </c>
     </row>
     <row r="37" spans="16:17" x14ac:dyDescent="0.25">
-      <c r="P37">
+      <c r="P37" s="1">
+        <v>100</v>
+      </c>
+      <c r="Q37" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="38" spans="16:17" x14ac:dyDescent="0.25">
+      <c r="P38" s="1">
         <v>110</v>
       </c>
-      <c r="Q37">
+      <c r="Q38" s="1">
         <v>3.5</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="P24:Q24"/>
+    <mergeCell ref="P5:Q5"/>
+    <mergeCell ref="E5:F5"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>